<commit_message>
Severity column was filled
</commit_message>
<xml_diff>
--- a/Compatibility/Compatibility.xlsx
+++ b/Compatibility/Compatibility.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51092FA-1322-4D01-9185-4A43B499B5DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D4E922-9E3E-4D63-A548-4C7B982DACEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Check-List and statistics" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
   <si>
     <t>Check-list for 'https://lawsonfenning.com/' site:</t>
   </si>
@@ -365,6 +365,12 @@
       </rPr>
       <t xml:space="preserve"> testing</t>
     </r>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -1754,7 +1760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -2249,15 +2255,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA0F8D9-D84D-4910-B3CF-4748EED93C79}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="28" customWidth="1"/>
     <col min="4" max="4" width="53.7109375" customWidth="1"/>
     <col min="5" max="5" width="44.85546875" customWidth="1"/>
@@ -2308,7 +2314,9 @@
       <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="C2" s="26" t="s">
         <v>35</v>
       </c>
@@ -2349,7 +2357,9 @@
       <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="C3" s="26" t="s">
         <v>35</v>
       </c>
@@ -2379,7 +2389,9 @@
       <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="14" t="s">
+        <v>60</v>
+      </c>
       <c r="C4" s="26" t="s">
         <v>35</v>
       </c>
@@ -2407,7 +2419,9 @@
     </row>
     <row r="5" spans="1:33" s="24" customFormat="1" ht="327.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="C5" s="26" t="s">
         <v>35</v>
       </c>

</xml_diff>